<commit_message>
update date thru may 21 2021
</commit_message>
<xml_diff>
--- a/Inputs/variants.xlsx
+++ b/Inputs/variants.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/GitHub/LEMMA-Forecasts/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D2D3C66-6543-004B-930F-B6A1174960FD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBA9ED73-866C-F043-B3D9-27B7DFEBE6F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3680" yWindow="1820" windowWidth="27640" windowHeight="16940" xr2:uid="{709315D1-E826-7745-85B7-AA2E5505B52E}"/>
   </bookViews>
@@ -410,7 +410,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -443,16 +443,16 @@
         <v>8</v>
       </c>
       <c r="B2" s="1">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="C2" s="1">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="E2" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F2" s="1">
         <v>0</v>
@@ -466,13 +466,13 @@
         <v>62</v>
       </c>
       <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>11</v>
+      </c>
+      <c r="E3">
         <v>3</v>
-      </c>
-      <c r="D3">
-        <v>14</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -483,16 +483,16 @@
         <v>0</v>
       </c>
       <c r="B4">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C4">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D4">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E4">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F4">
         <v>0</v>

</xml_diff>